<commit_message>
Fix zero values in financial model and improve template generation
</commit_message>
<xml_diff>
--- a/backend/data/templates/financial_model_template.xlsx
+++ b/backend/data/templates/financial_model_template.xlsx
@@ -2,43 +2,84 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Inputs" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Cash Flow" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rent Roll" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="Market_Rent">'Inputs'!$B$2</definedName>
-    <definedName name="Exit_Yield">'Inputs'!$B$3</definedName>
-    <definedName name="CPI_Growth">'Inputs'!$B$4</definedName>
+    <definedName name="Area">Inputs!$B$3</definedName>
+    <definedName name="Capex">Inputs!$B$10</definedName>
+    <definedName name="Entry_Yield">Inputs!$B$6</definedName>
+    <definedName name="Equity_Invested">Inputs!$B$16</definedName>
+    <definedName name="Exit_Yield">Inputs!$B$7</definedName>
+    <definedName name="Initial_Gross_Income">Inputs!$B$13</definedName>
+    <definedName name="Interest_Rate">Inputs!$B$9</definedName>
+    <definedName name="Loan_Amount">Inputs!$B$15</definedName>
+    <definedName name="LTV">Inputs!$B$8</definedName>
+    <definedName name="Market_Rent">Inputs!$B$2</definedName>
+    <definedName name="OpEx_Ratio">Inputs!$B$5</definedName>
+    <definedName name="Purchase_Price">Inputs!$B$14</definedName>
+    <definedName name="Rent_Growth">Inputs!$B$4</definedName>
   </definedNames>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="181029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00\x"/>
+  </numFmts>
+  <fonts count="4">
     <font>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <family val="3"/>
+      <b val="1"/>
+      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <family val="3"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <family val="3"/>
+      <sz val="9"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF366092"/>
+        <bgColor rgb="FF366092"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -46,15 +87,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -417,109 +497,935 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="25" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Parameter</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Value</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Unit</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Named Range</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Market Rent</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>85</v>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>EUR/sqm/yr</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>Market_Rent</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Leasable Area</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>10000</v>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>sqm</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>Area</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>Rent Growth</t>
+        </is>
+      </c>
+      <c r="B4" s="4" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>Rent_Growth</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>OpEx Ratio</t>
+        </is>
+      </c>
+      <c r="B5" s="4" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>OpEx_Ratio</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>Entry Yield</t>
+        </is>
+      </c>
+      <c r="B6" s="4" t="n">
+        <v>0.045</v>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>Entry_Yield</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>Exit Yield</t>
+        </is>
+      </c>
+      <c r="B7" s="4" t="n">
+        <v>0.0475</v>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>Exit_Yield</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>LTV</t>
+        </is>
+      </c>
+      <c r="B8" s="4" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>LTV</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>Interest Rate</t>
+        </is>
+      </c>
+      <c r="B9" s="4" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>Interest_Rate</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>Capex</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>Capex</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="5" t="inlineStr">
+        <is>
+          <t>Calculated Values</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Initial Gross Income</t>
+        </is>
+      </c>
+      <c r="B13">
+        <f>Market_Rent * Area</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Purchase Price</t>
+        </is>
+      </c>
+      <c r="B14">
+        <f>Initial_Gross_Income / Entry_Yield</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Loan Amount</t>
+        </is>
+      </c>
+      <c r="B15">
+        <f>Purchase_Price * LTV</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Equity Invested</t>
+        </is>
+      </c>
+      <c r="B16">
+        <f>Purchase_Price - Loan_Amount + Capex</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="25" customWidth="1" min="1" max="1"/>
+    <col width="14.33203125" customWidth="1" min="2" max="2"/>
+    <col width="18.109375" customWidth="1" min="3" max="3"/>
+    <col width="15.44140625" customWidth="1" min="4" max="4"/>
+    <col width="17.109375" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="14.88671875" customWidth="1" min="7" max="7"/>
+    <col width="14.5546875" customWidth="1" min="8" max="9"/>
+    <col width="12.88671875" customWidth="1" min="10" max="11"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Item</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Year 1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Year 6</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Year 7</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Year 8</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Year 9</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Year 10</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Market Rent (EUR/sqm)</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Market_Rent</t>
-        </is>
+          <t>Potential Gross Income</t>
+        </is>
+      </c>
+      <c r="B2" s="6">
+        <f>Initial_Gross_Income * (1 + Rent_Growth)^0</f>
+        <v/>
+      </c>
+      <c r="C2" s="6">
+        <f>Initial_Gross_Income * (1 + Rent_Growth)^1</f>
+        <v/>
+      </c>
+      <c r="D2" s="6">
+        <f>Initial_Gross_Income * (1 + Rent_Growth)^2</f>
+        <v/>
+      </c>
+      <c r="E2" s="6">
+        <f>Initial_Gross_Income * (1 + Rent_Growth)^3</f>
+        <v/>
+      </c>
+      <c r="F2" s="6">
+        <f>Initial_Gross_Income * (1 + Rent_Growth)^4</f>
+        <v/>
+      </c>
+      <c r="G2" s="6">
+        <f>Initial_Gross_Income * (1 + Rent_Growth)^5</f>
+        <v/>
+      </c>
+      <c r="H2" s="6">
+        <f>Initial_Gross_Income * (1 + Rent_Growth)^6</f>
+        <v/>
+      </c>
+      <c r="I2" s="6">
+        <f>Initial_Gross_Income * (1 + Rent_Growth)^7</f>
+        <v/>
+      </c>
+      <c r="J2" s="6">
+        <f>Initial_Gross_Income * (1 + Rent_Growth)^8</f>
+        <v/>
+      </c>
+      <c r="K2" s="6">
+        <f>Initial_Gross_Income * (1 + Rent_Growth)^9</f>
+        <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Exit Yield (%)</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Exit_Yield</t>
-        </is>
+          <t>Operating Expenses</t>
+        </is>
+      </c>
+      <c r="B3" s="6">
+        <f>-B2 * OpEx_Ratio</f>
+        <v/>
+      </c>
+      <c r="C3" s="6">
+        <f>-C2 * OpEx_Ratio</f>
+        <v/>
+      </c>
+      <c r="D3" s="6">
+        <f>-D2 * OpEx_Ratio</f>
+        <v/>
+      </c>
+      <c r="E3" s="6">
+        <f>-E2 * OpEx_Ratio</f>
+        <v/>
+      </c>
+      <c r="F3" s="6">
+        <f>-F2 * OpEx_Ratio</f>
+        <v/>
+      </c>
+      <c r="G3" s="6">
+        <f>-G2 * OpEx_Ratio</f>
+        <v/>
+      </c>
+      <c r="H3" s="6">
+        <f>-H2 * OpEx_Ratio</f>
+        <v/>
+      </c>
+      <c r="I3" s="6">
+        <f>-I2 * OpEx_Ratio</f>
+        <v/>
+      </c>
+      <c r="J3" s="6">
+        <f>-J2 * OpEx_Ratio</f>
+        <v/>
+      </c>
+      <c r="K3" s="6">
+        <f>-K2 * OpEx_Ratio</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="inlineStr">
+        <is>
+          <t>Net Operating Income (NOI)</t>
+        </is>
+      </c>
+      <c r="B4" s="7">
+        <f>SUM(B2:B3)</f>
+        <v/>
+      </c>
+      <c r="C4" s="7">
+        <f>SUM(C2:C3)</f>
+        <v/>
+      </c>
+      <c r="D4" s="7">
+        <f>SUM(D2:D3)</f>
+        <v/>
+      </c>
+      <c r="E4" s="7">
+        <f>SUM(E2:E3)</f>
+        <v/>
+      </c>
+      <c r="F4" s="7">
+        <f>SUM(F2:F3)</f>
+        <v/>
+      </c>
+      <c r="G4" s="7">
+        <f>SUM(G2:G3)</f>
+        <v/>
+      </c>
+      <c r="H4" s="7">
+        <f>SUM(H2:H3)</f>
+        <v/>
+      </c>
+      <c r="I4" s="7">
+        <f>SUM(I2:I3)</f>
+        <v/>
+      </c>
+      <c r="J4" s="7">
+        <f>SUM(J2:J3)</f>
+        <v/>
+      </c>
+      <c r="K4" s="7">
+        <f>SUM(K2:K3)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Debt Service</t>
+        </is>
+      </c>
+      <c r="B5" s="6">
+        <f>-Loan_Amount * Interest_Rate</f>
+        <v/>
+      </c>
+      <c r="C5" s="6">
+        <f>-Loan_Amount * Interest_Rate</f>
+        <v/>
+      </c>
+      <c r="D5" s="6">
+        <f>-Loan_Amount * Interest_Rate</f>
+        <v/>
+      </c>
+      <c r="E5" s="6">
+        <f>-Loan_Amount * Interest_Rate</f>
+        <v/>
+      </c>
+      <c r="F5" s="6">
+        <f>-Loan_Amount * Interest_Rate</f>
+        <v/>
+      </c>
+      <c r="G5" s="6">
+        <f>-Loan_Amount * Interest_Rate</f>
+        <v/>
+      </c>
+      <c r="H5" s="6">
+        <f>-Loan_Amount * Interest_Rate</f>
+        <v/>
+      </c>
+      <c r="I5" s="6">
+        <f>-Loan_Amount * Interest_Rate</f>
+        <v/>
+      </c>
+      <c r="J5" s="6">
+        <f>-Loan_Amount * Interest_Rate</f>
+        <v/>
+      </c>
+      <c r="K5" s="6">
+        <f>-Loan_Amount * Interest_Rate</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="inlineStr">
+        <is>
+          <t>Net Cash Flow</t>
+        </is>
+      </c>
+      <c r="B6" s="8">
+        <f>B4 + B5</f>
+        <v/>
+      </c>
+      <c r="C6" s="8">
+        <f>C4 + C5</f>
+        <v/>
+      </c>
+      <c r="D6" s="8">
+        <f>D4 + D5</f>
+        <v/>
+      </c>
+      <c r="E6" s="8">
+        <f>E4 + E5</f>
+        <v/>
+      </c>
+      <c r="F6" s="8">
+        <f>F4 + F5</f>
+        <v/>
+      </c>
+      <c r="G6" s="8">
+        <f>G4 + G5</f>
+        <v/>
+      </c>
+      <c r="H6" s="8">
+        <f>H4 + H5</f>
+        <v/>
+      </c>
+      <c r="I6" s="8">
+        <f>I4 + I5</f>
+        <v/>
+      </c>
+      <c r="J6" s="8">
+        <f>J4 + J5</f>
+        <v/>
+      </c>
+      <c r="K6" s="8">
+        <f>K4 + K5</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5" t="inlineStr">
+        <is>
+          <t>Exit Valuation (Year 10)</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Exit NOI (Forward)</t>
+        </is>
+      </c>
+      <c r="B9" s="6">
+        <f>L4 * (1+Rent_Growth)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Exit Value</t>
+        </is>
+      </c>
+      <c r="B10" s="6">
+        <f>B9 / Exit_Yield</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Loan Repayment</t>
+        </is>
+      </c>
+      <c r="B11" s="6">
+        <f>-Loan_Amount</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Net Sale Proceeds</t>
+        </is>
+      </c>
+      <c r="B12" s="8">
+        <f>SUM(B10:B11)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="5" t="inlineStr">
+        <is>
+          <t>Levered Cash Flow Stream</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Year 0</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Year 1</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Year 6</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Year 7</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Year 8</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Year 9</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Year 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="6">
+        <f>-Equity_Invested</f>
+        <v/>
+      </c>
+      <c r="C15" s="6">
+        <f>B6</f>
+        <v/>
+      </c>
+      <c r="D15" s="6">
+        <f>C6</f>
+        <v/>
+      </c>
+      <c r="E15" s="6">
+        <f>D6</f>
+        <v/>
+      </c>
+      <c r="F15" s="6">
+        <f>E6</f>
+        <v/>
+      </c>
+      <c r="G15" s="6">
+        <f>F6</f>
+        <v/>
+      </c>
+      <c r="H15" s="6">
+        <f>G6</f>
+        <v/>
+      </c>
+      <c r="I15" s="6">
+        <f>H6</f>
+        <v/>
+      </c>
+      <c r="J15" s="6">
+        <f>I6</f>
+        <v/>
+      </c>
+      <c r="K15" s="6">
+        <f>J6</f>
+        <v/>
+      </c>
+      <c r="L15" s="6">
+        <f>K6 + B12</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="5" t="inlineStr">
+        <is>
+          <t>Returns Metrics</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Levered IRR</t>
+        </is>
+      </c>
+      <c r="B18" s="9">
+        <f>IRR(B15:L15)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Equity Multiple</t>
+        </is>
+      </c>
+      <c r="B19" s="11">
+        <f>(SUM(C15:L15) + ABS(B15)) / ABS(B15)</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Tenant Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Unit</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Area (sqm)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Lease Start</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Lease End</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Annual Rent (EUR)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Rent/sqm/yr</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Logistics Corp A</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Unit 1</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2023-01-01</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2028-12-31</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>425000</v>
+      </c>
+      <c r="G2" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>E-Commerce Ltd</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Unit 2</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2024-06-01</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2029-05-31</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>270000</v>
+      </c>
+      <c r="G3" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CPI Growth (%)</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>CPI_Growth</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Purchase Price</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>5000000</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Purchase_Price</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Cap Rate</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Cap_Rate</t>
-        </is>
+          <t>Global Supply Chain</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Unit 3</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>2000</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2022-01-01</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2027-12-31</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>160000</v>
+      </c>
+      <c r="G4" t="n">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix IRR calculation logic and update fallback value
</commit_message>
<xml_diff>
--- a/backend/data/templates/financial_model_template.xlsx
+++ b/backend/data/templates/financial_model_template.xlsx
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="B2" s="3" t="n">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
@@ -637,7 +637,7 @@
         </is>
       </c>
       <c r="B7" s="4" t="n">
-        <v>0.0475</v>
+        <v>0.25</v>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Fix financial model inputs: sync market rent and extract asset area from JSON
</commit_message>
<xml_diff>
--- a/backend/data/templates/financial_model_template.xlsx
+++ b/backend/data/templates/financial_model_template.xlsx
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="B2" s="3" t="n">
-        <v>82</v>
+        <v>83.06</v>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
@@ -557,7 +557,7 @@
         </is>
       </c>
       <c r="B3" s="3" t="n">
-        <v>10000</v>
+        <v>222221</v>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Edit financial_model_template.xlsx to correct related data value
</commit_message>
<xml_diff>
--- a/backend/data/templates/financial_model_template.xlsx
+++ b/backend/data/templates/financial_model_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Inputs" sheetId="1" state="visible" r:id="rId1"/>
@@ -45,6 +45,7 @@
     <font>
       <name val="宋体"/>
       <charset val="134"/>
+      <family val="3"/>
       <b val="1"/>
       <color rgb="FFFFFFFF"/>
       <sz val="11"/>
@@ -52,6 +53,7 @@
     <font>
       <name val="宋体"/>
       <charset val="134"/>
+      <family val="3"/>
       <b val="1"/>
       <sz val="11"/>
     </font>
@@ -497,8 +499,8 @@
   </sheetPr>
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -774,8 +776,8 @@
   </sheetPr>
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -1099,7 +1101,7 @@
         </is>
       </c>
       <c r="B9" s="6">
-        <f>L4 * (1+Rent_Growth)</f>
+        <f>K4*(1+Rent_Growth)</f>
         <v/>
       </c>
     </row>
@@ -1110,7 +1112,7 @@
         </is>
       </c>
       <c r="B10" s="6">
-        <f>B9 / Exit_Yield</f>
+        <f>B9/Exit_Yield</f>
         <v/>
       </c>
     </row>
@@ -1258,7 +1260,7 @@
         </is>
       </c>
       <c r="B18" s="9">
-        <f>IRR(B15:K15)</f>
+        <f>IRR(B15:L15)</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix: Update Yield on Cost to use Year 1 NOI (B4) in both Python and Excel
</commit_message>
<xml_diff>
--- a/backend/data/templates/financial_model_template.xlsx
+++ b/backend/data/templates/financial_model_template.xlsx
@@ -777,7 +777,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -1282,7 +1282,7 @@
         </is>
       </c>
       <c r="B20" s="9">
-        <f>C4 / (Purchase_Price + Capex)</f>
+        <f>B4/(Purchase_Price+Capex)</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Update scenario analysis output format
</commit_message>
<xml_diff>
--- a/backend/data/templates/financial_model_template.xlsx
+++ b/backend/data/templates/financial_model_template.xlsx
@@ -539,7 +539,7 @@
         </is>
       </c>
       <c r="B2" s="3" t="n">
-        <v>5</v>
+        <v>80.5682</v>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
@@ -639,7 +639,7 @@
         </is>
       </c>
       <c r="B7" s="4" t="n">
-        <v>0.05</v>
+        <v>0.0485</v>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Enhance scenario analysis with semantic parsing and robust regex fallback
</commit_message>
<xml_diff>
--- a/backend/data/templates/financial_model_template.xlsx
+++ b/backend/data/templates/financial_model_template.xlsx
@@ -539,7 +539,7 @@
         </is>
       </c>
       <c r="B2" s="3" t="n">
-        <v>80.5682</v>
+        <v>78.907</v>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
@@ -639,7 +639,7 @@
         </is>
       </c>
       <c r="B7" s="4" t="n">
-        <v>0.0485</v>
+        <v>0.05</v>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update financial metric labels in output text
</commit_message>
<xml_diff>
--- a/backend/data/templates/financial_model_template.xlsx
+++ b/backend/data/templates/financial_model_template.xlsx
@@ -539,7 +539,7 @@
         </is>
       </c>
       <c r="B2" s="3" t="n">
-        <v>83.06</v>
+        <v>80.5682</v>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
@@ -619,7 +619,7 @@
         </is>
       </c>
       <c r="B6" s="4" t="n">
-        <v>0.045</v>
+        <v>0.05</v>
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
@@ -639,7 +639,7 @@
         </is>
       </c>
       <c r="B7" s="4" t="n">
-        <v>0.1225</v>
+        <v>0.046</v>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update scenario Excel format and add update message
</commit_message>
<xml_diff>
--- a/backend/data/templates/financial_model_template.xlsx
+++ b/backend/data/templates/financial_model_template.xlsx
@@ -539,7 +539,7 @@
         </is>
       </c>
       <c r="B2" s="3" t="n">
-        <v>80.5682</v>
+        <v>87.21300000000001</v>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
@@ -619,7 +619,7 @@
         </is>
       </c>
       <c r="B6" s="4" t="n">
-        <v>0.05</v>
+        <v>0.045</v>
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
@@ -639,7 +639,7 @@
         </is>
       </c>
       <c r="B7" s="4" t="n">
-        <v>0.046</v>
+        <v>0.05</v>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Improve LLM prompt for deal summary to avoid placeholders and technical jargon
</commit_message>
<xml_diff>
--- a/backend/data/templates/financial_model_template.xlsx
+++ b/backend/data/templates/financial_model_template.xlsx
@@ -539,7 +539,7 @@
         </is>
       </c>
       <c r="B2" s="3" t="n">
-        <v>87.21300000000001</v>
+        <v>83.06999999999999</v>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
@@ -639,7 +639,7 @@
         </is>
       </c>
       <c r="B7" s="4" t="n">
-        <v>0.05</v>
+        <v>0.0475</v>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Fix scenario parsing, PPT yields, UI links, and prompts
</commit_message>
<xml_diff>
--- a/backend/data/templates/financial_model_template.xlsx
+++ b/backend/data/templates/financial_model_template.xlsx
@@ -539,7 +539,7 @@
         </is>
       </c>
       <c r="B2" s="3" t="n">
-        <v>83.06999999999999</v>
+        <v>78.907</v>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
@@ -639,7 +639,7 @@
         </is>
       </c>
       <c r="B7" s="4" t="n">
-        <v>0.0475</v>
+        <v>0.05</v>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Fix scenario analysis data flow and deck generation logic
</commit_message>
<xml_diff>
--- a/backend/data/templates/financial_model_template.xlsx
+++ b/backend/data/templates/financial_model_template.xlsx
@@ -539,7 +539,7 @@
         </is>
       </c>
       <c r="B2" s="3" t="n">
-        <v>78.907</v>
+        <v>84.59661</v>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
@@ -639,7 +639,7 @@
         </is>
       </c>
       <c r="B7" s="4" t="n">
-        <v>0.05</v>
+        <v>0.051</v>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Generate comps mock data
</commit_message>
<xml_diff>
--- a/backend/data/templates/financial_model_template.xlsx
+++ b/backend/data/templates/financial_model_template.xlsx
@@ -539,7 +539,7 @@
         </is>
       </c>
       <c r="B2" s="3" t="n">
-        <v>84.59661</v>
+        <v>81.89710000000001</v>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
@@ -639,7 +639,7 @@
         </is>
       </c>
       <c r="B7" s="4" t="n">
-        <v>0.051</v>
+        <v>0.0485</v>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>

</xml_diff>